<commit_message>
check merge file and upload file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lap - 2203-0155\Documents\UiPath\Generate Yearly Report Peformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F490CE-FEC1-4B5A-8AFB-D48AC4D19F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291DA29E-8524-4164-B83B-EE77D1D56C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Data\Report\</t>
-  </si>
-  <si>
     <t>https://acme-test.uipath.com/reports/download</t>
   </si>
   <si>
@@ -209,6 +206,12 @@
   </si>
   <si>
     <t>.\Data\Output\status.xlsx</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items</t>
+  </si>
+  <si>
+    <t>Data\Output</t>
   </si>
 </sst>
 </file>
@@ -587,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -638,7 +641,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -649,7 +652,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -661,7 +664,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -671,8 +674,8 @@
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>50</v>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -680,7 +683,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -688,7 +691,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -696,7 +699,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -704,29 +707,31 @@
         <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
         <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>